<commit_message>
Added more interface memory
</commit_message>
<xml_diff>
--- a/rack_v2.0/PLC/type_B/data/global_variable_template.xlsx
+++ b/rack_v2.0/PLC/type_B/data/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1687" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1716" uniqueCount="897">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2463,9 +2463,6 @@
     <t>Control Shelf stage duration percentage</t>
   </si>
   <si>
-    <t>CTRL_pump_fill_drain_mode</t>
-  </si>
-  <si>
     <t>CTRL_pump_fill_mode_flowrate</t>
   </si>
   <si>
@@ -2674,6 +2671,63 @@
   </si>
   <si>
     <t>Type A(1), B(2), undefined(0)</t>
+  </si>
+  <si>
+    <t>D250.0</t>
+  </si>
+  <si>
+    <t>E-stop</t>
+  </si>
+  <si>
+    <t>FEEDBACK_ESTOP_Status</t>
+  </si>
+  <si>
+    <t>FEEDBACK_pump_rpm</t>
+  </si>
+  <si>
+    <t>FEEDBACK_pump_flowrate</t>
+  </si>
+  <si>
+    <t>D4180</t>
+  </si>
+  <si>
+    <t>RPM reading</t>
+  </si>
+  <si>
+    <t>Flowrate reading</t>
+  </si>
+  <si>
+    <t>D4183</t>
+  </si>
+  <si>
+    <t>D4186</t>
+  </si>
+  <si>
+    <t>Flowrate per shelf</t>
+  </si>
+  <si>
+    <t>REF_pump_flowrate_per_shelf_setpoint</t>
+  </si>
+  <si>
+    <t>Recovery from PID ramp up of pump due to low water</t>
+  </si>
+  <si>
+    <t>D4190.0</t>
+  </si>
+  <si>
+    <t>CTRL_pump_pid_recovery</t>
+  </si>
+  <si>
+    <t>FEEDBACK_pump_fill_drain_timer</t>
+  </si>
+  <si>
+    <t>D4192</t>
+  </si>
+  <si>
+    <t>Running timer for both fill and drain mode</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -3032,8 +3086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5407,8 +5461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5955,10 +6009,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G162"/>
+  <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8272,47 +8326,44 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>876</v>
+        <v>880</v>
       </c>
       <c r="B134" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C134" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D134">
         <v>0</v>
       </c>
       <c r="F134" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>815</v>
+        <v>875</v>
       </c>
       <c r="B135" t="s">
-        <v>508</v>
-      </c>
-      <c r="C135" s="8" t="s">
-        <v>605</v>
-      </c>
-      <c r="D135" t="s">
-        <v>606</v>
-      </c>
-      <c r="E135" t="s">
-        <v>133</v>
+        <v>876</v>
+      </c>
+      <c r="C135" t="s">
+        <v>1</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
       </c>
       <c r="F135" t="s">
-        <v>806</v>
+        <v>877</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>802</v>
+        <v>814</v>
       </c>
       <c r="B136" t="s">
-        <v>814</v>
+        <v>508</v>
       </c>
       <c r="C136" s="8" t="s">
         <v>605</v>
@@ -8324,15 +8375,15 @@
         <v>133</v>
       </c>
       <c r="F136" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>816</v>
+        <v>802</v>
       </c>
       <c r="B137" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="C137" s="8" t="s">
         <v>605</v>
@@ -8340,16 +8391,19 @@
       <c r="D137" t="s">
         <v>606</v>
       </c>
+      <c r="E137" t="s">
+        <v>133</v>
+      </c>
       <c r="F137" t="s">
-        <v>823</v>
+        <v>807</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>803</v>
+        <v>815</v>
       </c>
       <c r="B138" t="s">
-        <v>822</v>
+        <v>816</v>
       </c>
       <c r="C138" s="8" t="s">
         <v>605</v>
@@ -8358,66 +8412,66 @@
         <v>606</v>
       </c>
       <c r="F138" t="s">
-        <v>828</v>
+        <v>822</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>824</v>
+        <v>803</v>
       </c>
       <c r="B139" t="s">
-        <v>825</v>
-      </c>
-      <c r="C139" t="s">
-        <v>607</v>
+        <v>821</v>
+      </c>
+      <c r="C139" s="8" t="s">
+        <v>605</v>
       </c>
       <c r="D139" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F139" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>808</v>
+        <v>823</v>
       </c>
       <c r="B140" t="s">
-        <v>818</v>
+        <v>824</v>
       </c>
       <c r="C140" t="s">
-        <v>2</v>
+        <v>607</v>
       </c>
       <c r="D140" t="s">
-        <v>0</v>
+        <v>608</v>
       </c>
       <c r="F140" t="s">
-        <v>810</v>
+        <v>825</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
+        <v>896</v>
+      </c>
+      <c r="B141" t="s">
+        <v>817</v>
+      </c>
+      <c r="C141" t="s">
+        <v>2</v>
+      </c>
+      <c r="D141" t="s">
+        <v>0</v>
+      </c>
+      <c r="F141" t="s">
         <v>809</v>
-      </c>
-      <c r="B141" t="s">
-        <v>819</v>
-      </c>
-      <c r="C141" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D141" t="s">
-        <v>12</v>
-      </c>
-      <c r="F141" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="B142" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="C142" s="8" t="s">
         <v>11</v>
@@ -8426,15 +8480,15 @@
         <v>12</v>
       </c>
       <c r="F142" t="s">
-        <v>813</v>
+        <v>810</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>829</v>
+        <v>811</v>
       </c>
       <c r="B143" t="s">
-        <v>831</v>
+        <v>819</v>
       </c>
       <c r="C143" s="8" t="s">
         <v>11</v>
@@ -8443,15 +8497,15 @@
         <v>12</v>
       </c>
       <c r="F143" t="s">
-        <v>833</v>
+        <v>812</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>828</v>
+      </c>
+      <c r="B144" t="s">
         <v>830</v>
-      </c>
-      <c r="B144" t="s">
-        <v>821</v>
       </c>
       <c r="C144" s="8" t="s">
         <v>11</v>
@@ -8460,32 +8514,32 @@
         <v>12</v>
       </c>
       <c r="F144" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>835</v>
+        <v>829</v>
       </c>
       <c r="B145" t="s">
-        <v>832</v>
-      </c>
-      <c r="C145" t="s">
-        <v>2</v>
+        <v>820</v>
+      </c>
+      <c r="C145" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D145" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F145" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="B146" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
       <c r="C146" t="s">
         <v>2</v>
@@ -8494,66 +8548,66 @@
         <v>0</v>
       </c>
       <c r="F146" t="s">
-        <v>841</v>
+        <v>835</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>804</v>
+        <v>836</v>
       </c>
       <c r="B147" t="s">
         <v>838</v>
       </c>
       <c r="C147" t="s">
-        <v>607</v>
+        <v>2</v>
       </c>
       <c r="D147" t="s">
-        <v>608</v>
+        <v>0</v>
       </c>
       <c r="F147" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B148" t="s">
-        <v>840</v>
-      </c>
-      <c r="C148" s="8" t="s">
-        <v>605</v>
+        <v>837</v>
+      </c>
+      <c r="C148" t="s">
+        <v>607</v>
       </c>
       <c r="D148" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="F148" t="s">
-        <v>827</v>
+        <v>842</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>847</v>
+        <v>805</v>
       </c>
       <c r="B149" t="s">
-        <v>850</v>
+        <v>839</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>11</v>
+        <v>605</v>
       </c>
       <c r="D149" t="s">
-        <v>12</v>
+        <v>606</v>
       </c>
       <c r="F149" t="s">
-        <v>853</v>
+        <v>826</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B150" t="s">
-        <v>854</v>
+        <v>849</v>
       </c>
       <c r="C150" s="8" t="s">
         <v>11</v>
@@ -8562,15 +8616,15 @@
         <v>12</v>
       </c>
       <c r="F150" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="B151" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="C151" s="8" t="s">
         <v>11</v>
@@ -8579,32 +8633,32 @@
         <v>12</v>
       </c>
       <c r="F151" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>842</v>
+        <v>848</v>
       </c>
       <c r="B152" t="s">
-        <v>856</v>
-      </c>
-      <c r="C152" t="s">
-        <v>2</v>
+        <v>854</v>
+      </c>
+      <c r="C152" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="D152" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F152" t="s">
-        <v>845</v>
+        <v>851</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="B153" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="C153" t="s">
         <v>2</v>
@@ -8613,32 +8667,32 @@
         <v>0</v>
       </c>
       <c r="F153" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>860</v>
+        <v>843</v>
       </c>
       <c r="B154" t="s">
         <v>857</v>
       </c>
-      <c r="C154" s="8" t="s">
-        <v>611</v>
-      </c>
-      <c r="D154" s="7" t="s">
-        <v>612</v>
+      <c r="C154" t="s">
+        <v>2</v>
+      </c>
+      <c r="D154" t="s">
+        <v>0</v>
       </c>
       <c r="F154" t="s">
-        <v>231</v>
+        <v>845</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="B155" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="C155" s="8" t="s">
         <v>611</v>
@@ -8647,15 +8701,15 @@
         <v>612</v>
       </c>
       <c r="F155" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="B156" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="C156" s="8" t="s">
         <v>611</v>
@@ -8664,15 +8718,15 @@
         <v>612</v>
       </c>
       <c r="F156" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="B157" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C157" s="8" t="s">
         <v>611</v>
@@ -8681,15 +8735,15 @@
         <v>612</v>
       </c>
       <c r="F157" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="B158" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="C158" s="8" t="s">
         <v>611</v>
@@ -8698,15 +8752,15 @@
         <v>612</v>
       </c>
       <c r="F158" t="s">
-        <v>800</v>
+        <v>233</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="B159" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="C159" s="8" t="s">
         <v>611</v>
@@ -8715,15 +8769,15 @@
         <v>612</v>
       </c>
       <c r="F159" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>873</v>
+        <v>864</v>
       </c>
       <c r="B160" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="C160" s="8" t="s">
         <v>611</v>
@@ -8731,19 +8785,16 @@
       <c r="D160" s="7" t="s">
         <v>612</v>
       </c>
-      <c r="E160" t="s">
-        <v>133</v>
-      </c>
       <c r="F160" t="s">
-        <v>234</v>
+        <v>801</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="B161" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C161" s="8" t="s">
         <v>611</v>
@@ -8755,15 +8806,15 @@
         <v>133</v>
       </c>
       <c r="F161" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B162" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C162" s="8" t="s">
         <v>611</v>
@@ -8775,7 +8826,112 @@
         <v>133</v>
       </c>
       <c r="F162" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>874</v>
+      </c>
+      <c r="B163" t="s">
+        <v>871</v>
+      </c>
+      <c r="C163" s="8" t="s">
+        <v>611</v>
+      </c>
+      <c r="D163" s="7" t="s">
+        <v>612</v>
+      </c>
+      <c r="E163" t="s">
+        <v>133</v>
+      </c>
+      <c r="F163" t="s">
         <v>236</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>881</v>
+      </c>
+      <c r="B164" t="s">
+        <v>883</v>
+      </c>
+      <c r="C164" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D164" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F164" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>882</v>
+      </c>
+      <c r="B165" t="s">
+        <v>886</v>
+      </c>
+      <c r="C165" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D165" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F165" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>889</v>
+      </c>
+      <c r="B166" t="s">
+        <v>887</v>
+      </c>
+      <c r="C166" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D166" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F166" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>892</v>
+      </c>
+      <c r="B167" t="s">
+        <v>891</v>
+      </c>
+      <c r="C167" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D167" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F167" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>893</v>
+      </c>
+      <c r="B168" t="s">
+        <v>894</v>
+      </c>
+      <c r="C168" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D168" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F168" t="s">
+        <v>895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improvements. Fix flowrate and rev (Hz) units in the HMI and PLC.
</commit_message>
<xml_diff>
--- a/rack_v2.0/PLC/type_B/data/global_variable_template.xlsx
+++ b/rack_v2.0/PLC/type_B/data/global_variable_template.xlsx
@@ -6321,7 +6321,7 @@
   <dimension ref="A1:G206"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C143" sqref="C143"/>
+      <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8759,7 +8759,7 @@
         <v>1</v>
       </c>
       <c r="D139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E139" t="s">
         <v>133</v>

</xml_diff>

<commit_message>
Added pump overspeed check.
</commit_message>
<xml_diff>
--- a/rack_v2.0/PLC/type_B/data/global_variable_template.xlsx
+++ b/rack_v2.0/PLC/type_B/data/global_variable_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="14370" windowHeight="10500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1807" uniqueCount="938">
   <si>
     <t>[3(FALSE)]</t>
   </si>
@@ -2830,6 +2830,27 @@
   </si>
   <si>
     <t>Rack ID</t>
+  </si>
+  <si>
+    <t>REF_pump_spin_limit</t>
+  </si>
+  <si>
+    <t>REF_pump_spin_limit_shutdown_time</t>
+  </si>
+  <si>
+    <t>D4700</t>
+  </si>
+  <si>
+    <t>Pump overspin limit</t>
+  </si>
+  <si>
+    <t>D4705</t>
+  </si>
+  <si>
+    <t>Pump overspin limit time before shutdown</t>
+  </si>
+  <si>
+    <t>[3(10)]</t>
   </si>
 </sst>
 </file>
@@ -5767,8 +5788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6276,13 +6297,13 @@
         <v>468</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>45</v>
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
       </c>
       <c r="F27" t="s">
         <v>133</v>
@@ -6318,10 +6339,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G206"/>
+  <dimension ref="A1:G208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D139" sqref="D139"/>
+    <sheetView topLeftCell="A178" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D209" sqref="D209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10022,6 +10043,46 @@
       </c>
       <c r="F206" t="s">
         <v>921</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>931</v>
+      </c>
+      <c r="B207" t="s">
+        <v>933</v>
+      </c>
+      <c r="C207" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D207" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E207" t="s">
+        <v>133</v>
+      </c>
+      <c r="F207" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>932</v>
+      </c>
+      <c r="B208" t="s">
+        <v>935</v>
+      </c>
+      <c r="C208" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D208" s="7" t="s">
+        <v>937</v>
+      </c>
+      <c r="E208" t="s">
+        <v>133</v>
+      </c>
+      <c r="F208" t="s">
+        <v>936</v>
       </c>
     </row>
   </sheetData>

</xml_diff>